<commit_message>
dosen pembimbing utama TA
</commit_message>
<xml_diff>
--- a/raw/sapto_aps9.xlsx
+++ b/raw/sapto_aps9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\format-excel-sapto\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E44ED99-FEE0-498B-B915-8C6199E919B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C351EC97-B768-46C8-B923-6DA8FEF7EA28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="839" firstSheet="27" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" tabRatio="839" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -2520,6 +2520,12 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2535,17 +2541,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3006,62 +3006,62 @@
       <c r="Y1" s="2"/>
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
-      <c r="O2" s="143"/>
-      <c r="P2" s="143"/>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="143"/>
-      <c r="S2" s="143"/>
-      <c r="T2" s="143"/>
-      <c r="U2" s="143"/>
-      <c r="V2" s="143"/>
-      <c r="W2" s="143"/>
-      <c r="X2" s="143"/>
-      <c r="Y2" s="143"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="145"/>
+      <c r="K2" s="145"/>
+      <c r="L2" s="145"/>
+      <c r="M2" s="145"/>
+      <c r="N2" s="145"/>
+      <c r="O2" s="145"/>
+      <c r="P2" s="145"/>
+      <c r="Q2" s="145"/>
+      <c r="R2" s="145"/>
+      <c r="S2" s="145"/>
+      <c r="T2" s="145"/>
+      <c r="U2" s="145"/>
+      <c r="V2" s="145"/>
+      <c r="W2" s="145"/>
+      <c r="X2" s="145"/>
+      <c r="Y2" s="145"/>
     </row>
     <row r="3" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="144" t="s">
+      <c r="A3" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="144"/>
-      <c r="C3" s="144"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
-      <c r="O3" s="144"/>
-      <c r="P3" s="144"/>
-      <c r="Q3" s="144"/>
-      <c r="R3" s="144"/>
-      <c r="S3" s="144"/>
-      <c r="T3" s="144"/>
-      <c r="U3" s="144"/>
-      <c r="V3" s="144"/>
-      <c r="W3" s="144"/>
-      <c r="X3" s="144"/>
-      <c r="Y3" s="144"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="146"/>
+      <c r="M3" s="146"/>
+      <c r="N3" s="146"/>
+      <c r="O3" s="146"/>
+      <c r="P3" s="146"/>
+      <c r="Q3" s="146"/>
+      <c r="R3" s="146"/>
+      <c r="S3" s="146"/>
+      <c r="T3" s="146"/>
+      <c r="U3" s="146"/>
+      <c r="V3" s="146"/>
+      <c r="W3" s="146"/>
+      <c r="X3" s="146"/>
+      <c r="Y3" s="146"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -3102,23 +3102,23 @@
       <c r="G5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="145"/>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="145"/>
-      <c r="Q5" s="145"/>
-      <c r="R5" s="145"/>
-      <c r="S5" s="145"/>
-      <c r="T5" s="145"/>
-      <c r="U5" s="145"/>
-      <c r="V5" s="145"/>
-      <c r="W5" s="145"/>
-      <c r="X5" s="145"/>
+      <c r="H5" s="147"/>
+      <c r="I5" s="147"/>
+      <c r="J5" s="147"/>
+      <c r="K5" s="147"/>
+      <c r="L5" s="147"/>
+      <c r="M5" s="147"/>
+      <c r="N5" s="147"/>
+      <c r="O5" s="147"/>
+      <c r="P5" s="147"/>
+      <c r="Q5" s="147"/>
+      <c r="R5" s="147"/>
+      <c r="S5" s="147"/>
+      <c r="T5" s="147"/>
+      <c r="U5" s="147"/>
+      <c r="V5" s="147"/>
+      <c r="W5" s="147"/>
+      <c r="X5" s="147"/>
       <c r="Y5" s="9"/>
     </row>
     <row r="6" spans="1:25" s="7" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3160,13 +3160,13 @@
       <c r="G7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="146"/>
-      <c r="I7" s="146"/>
-      <c r="J7" s="146"/>
-      <c r="K7" s="146"/>
-      <c r="L7" s="146"/>
-      <c r="M7" s="146"/>
-      <c r="N7" s="146"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="141"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -3448,9 +3448,9 @@
       <c r="G17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H17" s="146"/>
-      <c r="I17" s="146"/>
-      <c r="J17" s="146"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="141"/>
+      <c r="J17" s="141"/>
       <c r="K17" s="11" t="str">
         <f>IF(H17="Minimum","Studi telah mendapt ijin pembukaan program studi baru. Pengajuan usulan akreditasi pertama","")</f>
         <v/>
@@ -3739,13 +3739,13 @@
       <c r="G27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="146"/>
-      <c r="I27" s="146"/>
-      <c r="J27" s="146"/>
-      <c r="K27" s="146"/>
-      <c r="L27" s="146"/>
-      <c r="M27" s="146"/>
-      <c r="N27" s="146"/>
+      <c r="H27" s="141"/>
+      <c r="I27" s="141"/>
+      <c r="J27" s="141"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="141"/>
+      <c r="M27" s="141"/>
+      <c r="N27" s="141"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -3797,11 +3797,11 @@
       <c r="G29" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H29" s="147">
+      <c r="H29" s="148">
         <v>43536</v>
       </c>
-      <c r="I29" s="147"/>
-      <c r="J29" s="147"/>
+      <c r="I29" s="148"/>
+      <c r="J29" s="148"/>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
@@ -3857,23 +3857,23 @@
       <c r="G31" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="145"/>
-      <c r="I31" s="145"/>
-      <c r="J31" s="145"/>
-      <c r="K31" s="145"/>
-      <c r="L31" s="145"/>
-      <c r="M31" s="145"/>
-      <c r="N31" s="145"/>
-      <c r="O31" s="145"/>
-      <c r="P31" s="145"/>
-      <c r="Q31" s="145"/>
-      <c r="R31" s="145"/>
-      <c r="S31" s="145"/>
-      <c r="T31" s="145"/>
-      <c r="U31" s="145"/>
-      <c r="V31" s="145"/>
-      <c r="W31" s="145"/>
-      <c r="X31" s="145"/>
+      <c r="H31" s="147"/>
+      <c r="I31" s="147"/>
+      <c r="J31" s="147"/>
+      <c r="K31" s="147"/>
+      <c r="L31" s="147"/>
+      <c r="M31" s="147"/>
+      <c r="N31" s="147"/>
+      <c r="O31" s="147"/>
+      <c r="P31" s="147"/>
+      <c r="Q31" s="147"/>
+      <c r="R31" s="147"/>
+      <c r="S31" s="147"/>
+      <c r="T31" s="147"/>
+      <c r="U31" s="147"/>
+      <c r="V31" s="147"/>
+      <c r="W31" s="147"/>
+      <c r="X31" s="147"/>
       <c r="Y31" s="9"/>
     </row>
     <row r="32" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3915,23 +3915,23 @@
       <c r="G33" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H33" s="148"/>
-      <c r="I33" s="148"/>
-      <c r="J33" s="148"/>
-      <c r="K33" s="148"/>
-      <c r="L33" s="148"/>
-      <c r="M33" s="148"/>
-      <c r="N33" s="148"/>
-      <c r="O33" s="148"/>
-      <c r="P33" s="148"/>
-      <c r="Q33" s="148"/>
-      <c r="R33" s="148"/>
-      <c r="S33" s="148"/>
-      <c r="T33" s="148"/>
-      <c r="U33" s="148"/>
-      <c r="V33" s="148"/>
-      <c r="W33" s="148"/>
-      <c r="X33" s="148"/>
+      <c r="H33" s="149"/>
+      <c r="I33" s="149"/>
+      <c r="J33" s="149"/>
+      <c r="K33" s="149"/>
+      <c r="L33" s="149"/>
+      <c r="M33" s="149"/>
+      <c r="N33" s="149"/>
+      <c r="O33" s="149"/>
+      <c r="P33" s="149"/>
+      <c r="Q33" s="149"/>
+      <c r="R33" s="149"/>
+      <c r="S33" s="149"/>
+      <c r="T33" s="149"/>
+      <c r="U33" s="149"/>
+      <c r="V33" s="149"/>
+      <c r="W33" s="149"/>
+      <c r="X33" s="149"/>
       <c r="Y33" s="9"/>
     </row>
     <row r="34" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4143,23 +4143,23 @@
       <c r="G41" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H41" s="146"/>
-      <c r="I41" s="146"/>
-      <c r="J41" s="146"/>
-      <c r="K41" s="146"/>
-      <c r="L41" s="146"/>
-      <c r="M41" s="146"/>
-      <c r="N41" s="146"/>
-      <c r="O41" s="146"/>
-      <c r="P41" s="146"/>
-      <c r="Q41" s="146"/>
-      <c r="R41" s="146"/>
-      <c r="S41" s="146"/>
-      <c r="T41" s="146"/>
-      <c r="U41" s="146"/>
-      <c r="V41" s="146"/>
-      <c r="W41" s="146"/>
-      <c r="X41" s="146"/>
+      <c r="H41" s="141"/>
+      <c r="I41" s="141"/>
+      <c r="J41" s="141"/>
+      <c r="K41" s="141"/>
+      <c r="L41" s="141"/>
+      <c r="M41" s="141"/>
+      <c r="N41" s="141"/>
+      <c r="O41" s="141"/>
+      <c r="P41" s="141"/>
+      <c r="Q41" s="141"/>
+      <c r="R41" s="141"/>
+      <c r="S41" s="141"/>
+      <c r="T41" s="141"/>
+      <c r="U41" s="141"/>
+      <c r="V41" s="141"/>
+      <c r="W41" s="141"/>
+      <c r="X41" s="141"/>
       <c r="Y41" s="9"/>
     </row>
     <row r="42" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4197,23 +4197,23 @@
       <c r="E43" s="9"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
-      <c r="H43" s="146"/>
-      <c r="I43" s="146"/>
-      <c r="J43" s="146"/>
-      <c r="K43" s="146"/>
-      <c r="L43" s="146"/>
-      <c r="M43" s="146"/>
-      <c r="N43" s="146"/>
-      <c r="O43" s="146"/>
-      <c r="P43" s="146"/>
-      <c r="Q43" s="146"/>
-      <c r="R43" s="146"/>
-      <c r="S43" s="146"/>
-      <c r="T43" s="146"/>
-      <c r="U43" s="146"/>
-      <c r="V43" s="146"/>
-      <c r="W43" s="146"/>
-      <c r="X43" s="146"/>
+      <c r="H43" s="141"/>
+      <c r="I43" s="141"/>
+      <c r="J43" s="141"/>
+      <c r="K43" s="141"/>
+      <c r="L43" s="141"/>
+      <c r="M43" s="141"/>
+      <c r="N43" s="141"/>
+      <c r="O43" s="141"/>
+      <c r="P43" s="141"/>
+      <c r="Q43" s="141"/>
+      <c r="R43" s="141"/>
+      <c r="S43" s="141"/>
+      <c r="T43" s="141"/>
+      <c r="U43" s="141"/>
+      <c r="V43" s="141"/>
+      <c r="W43" s="141"/>
+      <c r="X43" s="141"/>
       <c r="Y43" s="9"/>
     </row>
     <row r="44" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4251,12 +4251,12 @@
       <c r="E45" s="9"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="141" t="s">
+      <c r="H45" s="143" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="141"/>
-      <c r="J45" s="141"/>
-      <c r="K45" s="141"/>
+      <c r="I45" s="143"/>
+      <c r="J45" s="143"/>
+      <c r="K45" s="143"/>
       <c r="L45" s="19"/>
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
@@ -4266,10 +4266,10 @@
       <c r="R45" s="19"/>
       <c r="S45" s="19"/>
       <c r="T45" s="19"/>
-      <c r="U45" s="142" t="s">
+      <c r="U45" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="V45" s="142"/>
+      <c r="V45" s="144"/>
       <c r="W45" s="19"/>
       <c r="X45" s="19"/>
       <c r="Y45" s="9"/>
@@ -4313,13 +4313,13 @@
       <c r="G47" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H47" s="146"/>
-      <c r="I47" s="146"/>
-      <c r="J47" s="146"/>
-      <c r="K47" s="146"/>
-      <c r="L47" s="146"/>
-      <c r="M47" s="146"/>
-      <c r="N47" s="146"/>
+      <c r="H47" s="141"/>
+      <c r="I47" s="141"/>
+      <c r="J47" s="141"/>
+      <c r="K47" s="141"/>
+      <c r="L47" s="141"/>
+      <c r="M47" s="141"/>
+      <c r="N47" s="141"/>
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="11"/>
@@ -4371,16 +4371,16 @@
       <c r="G49" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H49" s="146"/>
-      <c r="I49" s="146"/>
-      <c r="J49" s="146"/>
-      <c r="K49" s="146"/>
-      <c r="L49" s="146"/>
-      <c r="M49" s="146"/>
-      <c r="N49" s="146"/>
-      <c r="O49" s="146"/>
-      <c r="P49" s="146"/>
-      <c r="Q49" s="146"/>
+      <c r="H49" s="141"/>
+      <c r="I49" s="141"/>
+      <c r="J49" s="141"/>
+      <c r="K49" s="141"/>
+      <c r="L49" s="141"/>
+      <c r="M49" s="141"/>
+      <c r="N49" s="141"/>
+      <c r="O49" s="141"/>
+      <c r="P49" s="141"/>
+      <c r="Q49" s="141"/>
       <c r="R49" s="11"/>
       <c r="S49" s="11"/>
       <c r="T49" s="11"/>
@@ -4429,15 +4429,15 @@
       <c r="G51" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H51" s="146"/>
-      <c r="I51" s="146"/>
-      <c r="J51" s="146"/>
-      <c r="K51" s="146"/>
-      <c r="L51" s="146"/>
-      <c r="M51" s="146"/>
-      <c r="N51" s="146"/>
-      <c r="O51" s="146"/>
-      <c r="P51" s="146"/>
+      <c r="H51" s="141"/>
+      <c r="I51" s="141"/>
+      <c r="J51" s="141"/>
+      <c r="K51" s="141"/>
+      <c r="L51" s="141"/>
+      <c r="M51" s="141"/>
+      <c r="N51" s="141"/>
+      <c r="O51" s="141"/>
+      <c r="P51" s="141"/>
       <c r="Q51" s="11"/>
       <c r="R51" s="11"/>
       <c r="S51" s="11"/>
@@ -4616,12 +4616,12 @@
       <c r="R57" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="S57" s="146"/>
-      <c r="T57" s="146"/>
-      <c r="U57" s="146"/>
-      <c r="V57" s="146"/>
-      <c r="W57" s="146"/>
-      <c r="X57" s="146"/>
+      <c r="S57" s="141"/>
+      <c r="T57" s="141"/>
+      <c r="U57" s="141"/>
+      <c r="V57" s="141"/>
+      <c r="W57" s="141"/>
+      <c r="X57" s="141"/>
       <c r="Y57" s="9"/>
     </row>
     <row r="58" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4676,12 +4676,12 @@
       <c r="R59" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="S59" s="149">
+      <c r="S59" s="142">
         <f ca="1">TODAY()</f>
-        <v>43997</v>
-      </c>
-      <c r="T59" s="149"/>
-      <c r="U59" s="149"/>
+        <v>44003</v>
+      </c>
+      <c r="T59" s="142"/>
+      <c r="U59" s="142"/>
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
@@ -4748,11 +4748,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="18">
-    <mergeCell ref="H47:N47"/>
-    <mergeCell ref="H49:Q49"/>
-    <mergeCell ref="H51:P51"/>
-    <mergeCell ref="S57:X57"/>
-    <mergeCell ref="S59:U59"/>
     <mergeCell ref="H45:K45"/>
     <mergeCell ref="U45:V45"/>
     <mergeCell ref="A2:Y2"/>
@@ -4766,6 +4761,11 @@
     <mergeCell ref="H33:X33"/>
     <mergeCell ref="H41:X41"/>
     <mergeCell ref="H43:X43"/>
+    <mergeCell ref="H47:N47"/>
+    <mergeCell ref="H49:Q49"/>
+    <mergeCell ref="H51:P51"/>
+    <mergeCell ref="S57:X57"/>
+    <mergeCell ref="S59:U59"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H27 H53 H51:I51 H49:I49 H47:I47 H43:I43 H29" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -4792,17 +4792,17 @@
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="3" customWidth="1"/>
     <col min="3" max="6" width="7.5703125" style="3" customWidth="1"/>
     <col min="7" max="10" width="7.7109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="21.28515625" style="3" customWidth="1"/>
@@ -5326,16 +5326,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="10">
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:I7"/>
     <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C21" xr:uid="{00000000-0002-0000-0A00-000000000000}">
@@ -12019,11 +12019,11 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="20">
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="A21:A22"/>
@@ -12034,11 +12034,11 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
@@ -12426,7 +12426,7 @@
   <sheetPr codeName="Sheet37"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
@@ -15902,6 +15902,11 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="13">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="F11:F12"/>
@@ -15910,11 +15915,6 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:G34 L14:L34" xr:uid="{00000000-0002-0000-0800-000000000000}">

</xml_diff>